<commit_message>
download asset schedule added
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/excel_files/asset_schedule.xlsx
+++ b/afar_project/csv_path/excel_files/asset_schedule.xlsx
@@ -628,16 +628,16 @@
         <v>3111072.93</v>
       </c>
       <c r="D4" t="n">
-        <v>4264</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>3115336.93</v>
+        <v>3111072.93</v>
       </c>
       <c r="F4" t="n">
         <v>1367021.79</v>
       </c>
       <c r="G4" t="n">
-        <v>1748315.14</v>
+        <v>1744051.14</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -648,13 +648,13 @@
         <v>1235426.37</v>
       </c>
       <c r="J4" t="n">
-        <v>174831.51</v>
+        <v>174405.11</v>
       </c>
       <c r="K4" t="n">
         <v>426448.72</v>
       </c>
       <c r="L4" t="n">
-        <v>983809.16</v>
+        <v>983382.76</v>
       </c>
       <c r="M4" t="n">
         <v>2587.59</v>
@@ -663,7 +663,7 @@
         <v>2587.59</v>
       </c>
       <c r="O4" t="n">
-        <v>761918.39</v>
+        <v>758080.79</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -684,16 +684,16 @@
         <v>334523</v>
       </c>
       <c r="D5" t="n">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>334635</v>
+        <v>334523</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>334635</v>
+        <v>334523</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -704,13 +704,13 @@
         <v>236352.14</v>
       </c>
       <c r="J5" t="n">
-        <v>47805</v>
+        <v>47789</v>
       </c>
       <c r="K5" t="n">
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>284157.14</v>
+        <v>284141.14</v>
       </c>
       <c r="M5" t="n">
         <v>0.03</v>
@@ -719,7 +719,7 @@
         <v>0.03</v>
       </c>
       <c r="O5" t="n">
-        <v>50477.83</v>
+        <v>50381.83</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>

</xml_diff>